<commit_message>
Update words.xlsx with new data
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14380500-555A-4FEA-A0AF-CFE7783CE806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EF6ABC-64D6-4EE2-AA0A-18D1136F8783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="1003">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3103,6 +3103,22 @@
   </si>
   <si>
     <t>ほうそう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>選手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>せんしゅ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>代表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>だいひょう</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3512,10 +3528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F465"/>
+  <dimension ref="A1:F467"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
-      <selection activeCell="B465" sqref="B465"/>
+      <selection activeCell="A468" sqref="A468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8684,6 +8700,22 @@
         <v>998</v>
       </c>
     </row>
+    <row r="466" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A466" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="B466" s="3" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A467" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B467" s="3" t="s">
+        <v>1002</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>